<commit_message>
fix sro image file on each sheet
</commit_message>
<xml_diff>
--- a/templates/driver_master.xlsx
+++ b/templates/driver_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanwoo/projects/sro_sign_in/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3D80D0-4B2D-3F4C-B102-2C885C01B00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEC24D8-F724-B247-83DE-CEB9C4580B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{09AE6B6F-CB89-AB49-80A1-44011AF81147}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{09AE6B6F-CB89-AB49-80A1-44011AF81147}"/>
   </bookViews>
   <sheets>
     <sheet name="GTWCA" sheetId="2" r:id="rId1"/>
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="49" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -401,6 +401,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="48"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -758,7 +764,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1053,8 +1059,371 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="46" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="47" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="27" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="27" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="27" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="37" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="36" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="40" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="40" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="40" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1065,368 +1434,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="43" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="45" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="43" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="46" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="43" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="47" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="43" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="45" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="45" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="27" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="27" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="26" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="26" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="26" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="27" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="37" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="36" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="40" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1438,166 +1448,12 @@
   <dxfs count="40">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="20"/>
+        <sz val="12"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1660,35 +1516,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1744,112 +1571,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1978,6 +1699,112 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <top style="thin">
           <color rgb="FF000000"/>
@@ -2333,6 +2160,189 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2493,60 +2503,49 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>108857</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3585388</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>163285</xdr:rowOff>
+      <xdr:colOff>3556000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>120952</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{905E5C3B-08E1-F047-B439-A22AC32C67F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51F64D2D-74AC-FEE1-4D51-1A638EEB36E0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="13226143" y="308428"/>
-          <a:ext cx="3422102" cy="1215571"/>
+          <a:off x="13062857" y="199571"/>
+          <a:ext cx="3556000" cy="1481667"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2609,60 +2608,49 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>222807</xdr:colOff>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>133684</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3547237</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>133684</xdr:rowOff>
+      <xdr:colOff>3698875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>17546</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{503204E1-A08B-B64C-B4AA-90ACC7042013}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C686B309-8481-244F-AD21-858FF8F4AFC7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="17668596" y="133684"/>
-          <a:ext cx="3324430" cy="1180877"/>
+          <a:off x="17573625" y="0"/>
+          <a:ext cx="3556000" cy="1446296"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2835,59 +2823,59 @@
     <sortCondition ref="A9:A21"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="10" xr3:uid="{64A00265-0137-244B-A879-755DB86AB37A}" name="Car #" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{E1AB06A9-49A1-A342-85E2-94E454D24D73}" name="Team " dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{5F991BA1-917F-C243-890F-989FD97F57A4}" name="Driver 1" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{7B193668-8E5E-A946-841B-57E2D3220E7F}" name="Signature" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{7DBBB12C-91F5-F84F-9877-64EB480C31A9}" name="Driver 2" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{A564E557-0D01-C448-ABEF-1462F6CD056C}" name="Signature2" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{64A00265-0137-244B-A879-755DB86AB37A}" name="Car #" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{E1AB06A9-49A1-A342-85E2-94E454D24D73}" name="Team " dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{5F991BA1-917F-C243-890F-989FD97F57A4}" name="Driver 1" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{7B193668-8E5E-A946-841B-57E2D3220E7F}" name="Signature" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{7DBBB12C-91F5-F84F-9877-64EB480C31A9}" name="Driver 2" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{A564E557-0D01-C448-ABEF-1462F6CD056C}" name="Signature2" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46D306FC-0764-1348-B92E-2B04BFF7CD56}" name="Table2267" displayName="Table2267" ref="A7:F50" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46D306FC-0764-1348-B92E-2B04BFF7CD56}" name="Table2267" displayName="Table2267" ref="A7:F50" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:F42">
     <sortCondition ref="A11:A42"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="10" xr3:uid="{952FB897-24E6-FE43-9F1F-49F7E304DAA0}" name="Car #" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{1E3D7F2D-9B6A-3F41-8B6A-24DB7B4AFDCA}" name="Team " dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{91361E21-E1DB-DD43-A7EF-DDC7B2BF10C8}" name="Driver 1" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{28E91684-E101-4742-8F3B-82930E2D64B1}" name="Signature" dataDxfId="25"/>
-    <tableColumn id="12" xr3:uid="{817E82D4-7BAC-8347-99C5-4C65EF00E4BD}" name="Driver 2" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{BAC158D9-B709-2643-B1A7-7893A6EF7D6A}" name="Signature 2" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{952FB897-24E6-FE43-9F1F-49F7E304DAA0}" name="Car #" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{1E3D7F2D-9B6A-3F41-8B6A-24DB7B4AFDCA}" name="Team " dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{91361E21-E1DB-DD43-A7EF-DDC7B2BF10C8}" name="Driver 1" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{28E91684-E101-4742-8F3B-82930E2D64B1}" name="Signature" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{817E82D4-7BAC-8347-99C5-4C65EF00E4BD}" name="Driver 2" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{BAC158D9-B709-2643-B1A7-7893A6EF7D6A}" name="Signature 2" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F40C26F3-15F2-734B-91D7-024115DB378F}" name="Table2268" displayName="Table2268" ref="A7:D36" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F40C26F3-15F2-734B-91D7-024115DB378F}" name="Table2268" displayName="Table2268" ref="A7:D36" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D32">
     <sortCondition ref="A8:A32"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="10" xr3:uid="{3FE9C849-A77D-8D4C-90A0-016088813F73}" name="Car #" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{D7E2A6BF-AE71-F644-9478-8161C6716A46}" name="Team" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{2EE9EE97-2512-0E4C-A419-2F49AE212BC6}" name="Driver" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{DBBF9C78-BA38-564F-B05D-CF456385A7CB}" name="Signature" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{3FE9C849-A77D-8D4C-90A0-016088813F73}" name="Car #" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{D7E2A6BF-AE71-F644-9478-8161C6716A46}" name="Team" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{2EE9EE97-2512-0E4C-A419-2F49AE212BC6}" name="Driver" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{DBBF9C78-BA38-564F-B05D-CF456385A7CB}" name="Signature" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C41BE30A-3069-B640-891C-4A0475598B92}" name="Table226" displayName="Table226" ref="A7:D38" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C41BE30A-3069-B640-891C-4A0475598B92}" name="Table226" displayName="Table226" ref="A7:D38" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D28">
     <sortCondition ref="A7:A28"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="10" xr3:uid="{D3F1DE7F-9DCD-7F48-956D-BA537B4780CE}" name="Car #" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{39221AC8-AE14-C74E-BB8D-CE6CDED73BC6}" name="Team" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{938E642D-BE25-564E-A3A6-EA08E4799EA6}" name="Driver" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{3607B339-BEB4-A242-AA13-DCDBC8C22B7A}" name="Signature" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{D3F1DE7F-9DCD-7F48-956D-BA537B4780CE}" name="Car #" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{39221AC8-AE14-C74E-BB8D-CE6CDED73BC6}" name="Team" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{938E642D-BE25-564E-A3A6-EA08E4799EA6}" name="Driver" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{3607B339-BEB4-A242-AA13-DCDBC8C22B7A}" name="Signature" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3195,8 +3183,8 @@
   </sheetPr>
   <dimension ref="A2:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView view="pageLayout" zoomScale="70" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3213,24 +3201,25 @@
   <sheetData>
     <row r="2" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="222" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="2"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="223"/>
     </row>
     <row r="3" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="2"/>
+      <c r="C3" s="222"/>
+      <c r="D3" s="222"/>
+      <c r="E3" s="222"/>
+      <c r="F3" s="223"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="C4" s="222"/>
+      <c r="D4" s="222"/>
+      <c r="E4" s="222"/>
+      <c r="F4" s="223"/>
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="E5" s="4"/>
@@ -3256,170 +3245,171 @@
       </c>
     </row>
     <row r="8" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="215"/>
-      <c r="B8" s="109"/>
-      <c r="C8" s="110"/>
-      <c r="D8" s="110"/>
-      <c r="E8" s="216"/>
+      <c r="A8" s="210"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="211"/>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="217"/>
-      <c r="B9" s="110"/>
-      <c r="C9" s="194"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="110"/>
+      <c r="A9" s="212"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="189"/>
+      <c r="D9" s="189"/>
+      <c r="E9" s="105"/>
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="217"/>
-      <c r="B10" s="196"/>
-      <c r="C10" s="109"/>
-      <c r="D10" s="109"/>
-      <c r="E10" s="110"/>
+      <c r="A10" s="212"/>
+      <c r="B10" s="191"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="105"/>
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="215"/>
-      <c r="B11" s="109"/>
-      <c r="C11" s="109"/>
-      <c r="D11" s="109"/>
-      <c r="E11" s="218"/>
+      <c r="A11" s="210"/>
+      <c r="B11" s="104"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="213"/>
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="215"/>
-      <c r="B12" s="196"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="110"/>
+      <c r="A12" s="210"/>
+      <c r="B12" s="191"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="104"/>
+      <c r="E12" s="105"/>
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="215"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
+      <c r="A13" s="210"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="215"/>
-      <c r="B14" s="109"/>
-      <c r="C14" s="109"/>
-      <c r="D14" s="109"/>
-      <c r="E14" s="110"/>
+      <c r="A14" s="210"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="105"/>
       <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="217"/>
-      <c r="B15" s="109"/>
-      <c r="C15" s="109"/>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
+      <c r="A15" s="212"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
       <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="215"/>
-      <c r="B16" s="218"/>
-      <c r="C16" s="212"/>
-      <c r="D16" s="212"/>
-      <c r="E16" s="212"/>
+      <c r="A16" s="210"/>
+      <c r="B16" s="213"/>
+      <c r="C16" s="207"/>
+      <c r="D16" s="207"/>
+      <c r="E16" s="207"/>
       <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="219"/>
-      <c r="B17" s="220"/>
-      <c r="C17" s="221"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="212"/>
+      <c r="A17" s="214"/>
+      <c r="B17" s="215"/>
+      <c r="C17" s="216"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="207"/>
       <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="217"/>
-      <c r="B18" s="196"/>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="110"/>
+      <c r="A18" s="212"/>
+      <c r="B18" s="191"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="105"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="217"/>
-      <c r="B19" s="222"/>
-      <c r="C19" s="223"/>
-      <c r="D19" s="109"/>
-      <c r="E19" s="216"/>
+      <c r="A19" s="212"/>
+      <c r="B19" s="217"/>
+      <c r="C19" s="218"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="211"/>
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" s="6" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="217"/>
-      <c r="B20" s="110"/>
-      <c r="C20" s="110"/>
-      <c r="D20" s="110"/>
-      <c r="E20" s="212"/>
+      <c r="A20" s="212"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="207"/>
       <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:6" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="217"/>
-      <c r="B21" s="109"/>
-      <c r="C21" s="109"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="110"/>
+      <c r="A21" s="212"/>
+      <c r="B21" s="104"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="105"/>
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="224"/>
-      <c r="B22" s="212"/>
-      <c r="C22" s="225"/>
-      <c r="D22" s="212"/>
-      <c r="E22" s="226"/>
+      <c r="A22" s="219"/>
+      <c r="B22" s="207"/>
+      <c r="C22" s="220"/>
+      <c r="D22" s="207"/>
+      <c r="E22" s="221"/>
       <c r="F22" s="79"/>
     </row>
     <row r="23" spans="1:6" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="224"/>
-      <c r="B23" s="212"/>
-      <c r="C23" s="212"/>
-      <c r="D23" s="212"/>
-      <c r="E23" s="110"/>
+      <c r="A23" s="219"/>
+      <c r="B23" s="207"/>
+      <c r="C23" s="207"/>
+      <c r="D23" s="207"/>
+      <c r="E23" s="105"/>
       <c r="F23" s="79"/>
     </row>
     <row r="24" spans="1:6" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="224"/>
-      <c r="B24" s="212"/>
-      <c r="C24" s="212"/>
-      <c r="D24" s="212"/>
-      <c r="E24" s="110"/>
+      <c r="A24" s="219"/>
+      <c r="B24" s="207"/>
+      <c r="C24" s="207"/>
+      <c r="D24" s="207"/>
+      <c r="E24" s="105"/>
       <c r="F24" s="79"/>
     </row>
     <row r="25" spans="1:6" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="224"/>
-      <c r="B25" s="212"/>
-      <c r="C25" s="212"/>
-      <c r="D25" s="212"/>
-      <c r="E25" s="110"/>
+      <c r="A25" s="219"/>
+      <c r="B25" s="207"/>
+      <c r="C25" s="207"/>
+      <c r="D25" s="207"/>
+      <c r="E25" s="105"/>
       <c r="F25" s="79"/>
     </row>
     <row r="26" spans="1:6" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="224"/>
-      <c r="B26" s="212"/>
-      <c r="C26" s="212"/>
-      <c r="D26" s="212"/>
-      <c r="E26" s="110" t="s">
+      <c r="A26" s="219"/>
+      <c r="B26" s="207"/>
+      <c r="C26" s="207"/>
+      <c r="D26" s="207"/>
+      <c r="E26" s="105" t="s">
         <v>7</v>
       </c>
       <c r="F26" s="79"/>
     </row>
     <row r="27" spans="1:6" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="114"/>
-      <c r="B27" s="214"/>
-      <c r="C27" s="214"/>
-      <c r="D27" s="214"/>
-      <c r="E27" s="113"/>
+      <c r="A27" s="109"/>
+      <c r="B27" s="209"/>
+      <c r="C27" s="209"/>
+      <c r="D27" s="209"/>
+      <c r="E27" s="108"/>
       <c r="F27" s="82"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3438,14 +3428,14 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A22" zoomScale="57" zoomScaleNormal="115" zoomScalePageLayoutView="57" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="53.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="50.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="64" style="1" customWidth="1"/>
@@ -3454,28 +3444,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="222" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
     </row>
     <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
+      <c r="C3" s="222"/>
+      <c r="D3" s="222"/>
+      <c r="E3" s="222"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="C4" s="222"/>
+      <c r="D4" s="222"/>
+      <c r="E4" s="222"/>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="E5" s="4"/>
@@ -3504,323 +3494,323 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="48.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="115"/>
-      <c r="B8" s="116"/>
-      <c r="C8" s="117"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="116"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="112"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="111"/>
       <c r="F8" s="85"/>
     </row>
     <row r="9" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="115"/>
-      <c r="B9" s="116"/>
-      <c r="C9" s="117"/>
-      <c r="D9" s="118"/>
-      <c r="E9" s="116"/>
+      <c r="A9" s="110"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="111"/>
       <c r="F9" s="85"/>
     </row>
     <row r="10" spans="1:9" s="16" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="119"/>
-      <c r="B10" s="120"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="121"/>
+      <c r="A10" s="114"/>
+      <c r="B10" s="115"/>
+      <c r="C10" s="115"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="116"/>
       <c r="F10" s="86"/>
     </row>
     <row r="11" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="122"/>
-      <c r="B11" s="123"/>
-      <c r="C11" s="124"/>
-      <c r="D11" s="123"/>
-      <c r="E11" s="123"/>
+      <c r="A11" s="117"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="119"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="118"/>
       <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="125"/>
-      <c r="B12" s="126"/>
-      <c r="C12" s="126"/>
-      <c r="D12" s="127"/>
-      <c r="E12" s="128"/>
+      <c r="A12" s="120"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="121"/>
+      <c r="D12" s="122"/>
+      <c r="E12" s="123"/>
       <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="129"/>
-      <c r="B13" s="130"/>
-      <c r="C13" s="131"/>
-      <c r="D13" s="131"/>
-      <c r="E13" s="132"/>
+      <c r="A13" s="124"/>
+      <c r="B13" s="125"/>
+      <c r="C13" s="126"/>
+      <c r="D13" s="126"/>
+      <c r="E13" s="127"/>
       <c r="F13" s="87"/>
     </row>
     <row r="14" spans="1:9" s="17" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="115"/>
-      <c r="B14" s="133"/>
-      <c r="C14" s="124"/>
-      <c r="D14" s="132"/>
-      <c r="E14" s="116"/>
+      <c r="A14" s="110"/>
+      <c r="B14" s="128"/>
+      <c r="C14" s="119"/>
+      <c r="D14" s="127"/>
+      <c r="E14" s="111"/>
       <c r="F14" s="85"/>
     </row>
     <row r="15" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="134"/>
-      <c r="B15" s="123"/>
-      <c r="C15" s="124"/>
-      <c r="D15" s="124"/>
-      <c r="E15" s="123"/>
+      <c r="A15" s="129"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="118"/>
       <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:9" s="16" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="135"/>
-      <c r="B16" s="136"/>
-      <c r="C16" s="137"/>
-      <c r="D16" s="138"/>
-      <c r="E16" s="139"/>
+      <c r="A16" s="130"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="133"/>
+      <c r="E16" s="134"/>
       <c r="F16" s="88"/>
     </row>
     <row r="17" spans="1:6" s="16" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="135"/>
-      <c r="B17" s="136"/>
-      <c r="C17" s="137"/>
-      <c r="D17" s="140"/>
-      <c r="E17" s="139"/>
+      <c r="A17" s="130"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="132"/>
+      <c r="D17" s="135"/>
+      <c r="E17" s="134"/>
       <c r="F17" s="88"/>
     </row>
     <row r="18" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="141"/>
-      <c r="B18" s="123"/>
-      <c r="C18" s="124"/>
-      <c r="D18" s="123"/>
-      <c r="E18" s="123"/>
+      <c r="A18" s="136"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
       <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="141"/>
-      <c r="B19" s="123"/>
-      <c r="C19" s="123"/>
-      <c r="D19" s="123"/>
-      <c r="E19" s="123"/>
+      <c r="A19" s="136"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
       <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="141"/>
-      <c r="B20" s="123"/>
-      <c r="C20" s="124"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="124"/>
+      <c r="A20" s="136"/>
+      <c r="B20" s="118"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="118"/>
+      <c r="E20" s="119"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="142"/>
-      <c r="B21" s="143"/>
-      <c r="C21" s="143"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="144"/>
+      <c r="A21" s="137"/>
+      <c r="B21" s="138"/>
+      <c r="C21" s="138"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="139"/>
       <c r="F21" s="85"/>
     </row>
     <row r="22" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="145"/>
-      <c r="B22" s="123"/>
-      <c r="C22" s="124"/>
-      <c r="D22" s="124"/>
-      <c r="E22" s="123"/>
+      <c r="A22" s="140"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="118"/>
       <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="134"/>
-      <c r="B23" s="123"/>
-      <c r="C23" s="146"/>
-      <c r="D23" s="146"/>
-      <c r="E23" s="123"/>
+      <c r="A23" s="129"/>
+      <c r="B23" s="118"/>
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="118"/>
       <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="141"/>
-      <c r="B24" s="123"/>
-      <c r="C24" s="124"/>
-      <c r="D24" s="123"/>
-      <c r="E24" s="123"/>
+      <c r="A24" s="136"/>
+      <c r="B24" s="118"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="147"/>
-      <c r="B25" s="148"/>
-      <c r="C25" s="149"/>
-      <c r="D25" s="150"/>
-      <c r="E25" s="148"/>
+      <c r="A25" s="142"/>
+      <c r="B25" s="143"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="145"/>
+      <c r="E25" s="143"/>
       <c r="F25" s="89"/>
     </row>
     <row r="26" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="134"/>
-      <c r="B26" s="148"/>
-      <c r="C26" s="151"/>
-      <c r="D26" s="148"/>
-      <c r="E26" s="151"/>
+      <c r="A26" s="129"/>
+      <c r="B26" s="143"/>
+      <c r="C26" s="146"/>
+      <c r="D26" s="143"/>
+      <c r="E26" s="146"/>
       <c r="F26" s="90"/>
     </row>
     <row r="27" spans="1:6" s="16" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="135"/>
-      <c r="B27" s="136"/>
-      <c r="C27" s="136"/>
-      <c r="D27" s="136"/>
-      <c r="E27" s="152"/>
+      <c r="A27" s="130"/>
+      <c r="B27" s="131"/>
+      <c r="C27" s="131"/>
+      <c r="D27" s="131"/>
+      <c r="E27" s="147"/>
       <c r="F27" s="88"/>
     </row>
     <row r="28" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="134"/>
-      <c r="B28" s="124"/>
-      <c r="C28" s="124"/>
-      <c r="D28" s="124"/>
-      <c r="E28" s="123"/>
+      <c r="A28" s="129"/>
+      <c r="B28" s="119"/>
+      <c r="C28" s="119"/>
+      <c r="D28" s="119"/>
+      <c r="E28" s="118"/>
       <c r="F28" s="10"/>
     </row>
     <row r="29" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="134"/>
-      <c r="B29" s="123"/>
-      <c r="C29" s="123"/>
-      <c r="D29" s="123"/>
-      <c r="E29" s="153"/>
+      <c r="A29" s="129"/>
+      <c r="B29" s="118"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="118"/>
+      <c r="E29" s="148"/>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="134"/>
-      <c r="B30" s="123"/>
-      <c r="C30" s="124"/>
-      <c r="D30" s="124"/>
-      <c r="E30" s="154"/>
+      <c r="A30" s="129"/>
+      <c r="B30" s="118"/>
+      <c r="C30" s="119"/>
+      <c r="D30" s="119"/>
+      <c r="E30" s="149"/>
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="145"/>
-      <c r="B31" s="123"/>
-      <c r="C31" s="123"/>
-      <c r="D31" s="124"/>
-      <c r="E31" s="123"/>
+      <c r="A31" s="140"/>
+      <c r="B31" s="118"/>
+      <c r="C31" s="118"/>
+      <c r="D31" s="119"/>
+      <c r="E31" s="118"/>
       <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="155"/>
-      <c r="B32" s="124"/>
-      <c r="C32" s="124"/>
-      <c r="D32" s="124"/>
-      <c r="E32" s="123"/>
+      <c r="A32" s="150"/>
+      <c r="B32" s="119"/>
+      <c r="C32" s="119"/>
+      <c r="D32" s="119"/>
+      <c r="E32" s="118"/>
       <c r="F32" s="10"/>
     </row>
     <row r="33" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="156"/>
-      <c r="B33" s="123"/>
-      <c r="C33" s="123"/>
-      <c r="D33" s="132"/>
-      <c r="E33" s="123"/>
+      <c r="A33" s="151"/>
+      <c r="B33" s="118"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="127"/>
+      <c r="E33" s="118"/>
       <c r="F33" s="19"/>
     </row>
     <row r="34" spans="1:6" s="16" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="135"/>
-      <c r="B34" s="136"/>
-      <c r="C34" s="137"/>
-      <c r="D34" s="120"/>
-      <c r="E34" s="139"/>
+      <c r="A34" s="130"/>
+      <c r="B34" s="131"/>
+      <c r="C34" s="132"/>
+      <c r="D34" s="115"/>
+      <c r="E34" s="134"/>
       <c r="F34" s="88"/>
     </row>
     <row r="35" spans="1:6" s="16" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="135"/>
-      <c r="B35" s="136"/>
-      <c r="C35" s="136"/>
-      <c r="D35" s="138"/>
-      <c r="E35" s="139"/>
+      <c r="A35" s="130"/>
+      <c r="B35" s="131"/>
+      <c r="C35" s="131"/>
+      <c r="D35" s="133"/>
+      <c r="E35" s="134"/>
       <c r="F35" s="88"/>
     </row>
     <row r="36" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="147"/>
-      <c r="B36" s="123"/>
-      <c r="C36" s="124"/>
-      <c r="D36" s="131"/>
-      <c r="E36" s="116"/>
+      <c r="A36" s="142"/>
+      <c r="B36" s="118"/>
+      <c r="C36" s="119"/>
+      <c r="D36" s="126"/>
+      <c r="E36" s="111"/>
       <c r="F36" s="85"/>
     </row>
     <row r="37" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="134"/>
-      <c r="B37" s="124"/>
-      <c r="C37" s="124"/>
-      <c r="D37" s="124"/>
-      <c r="E37" s="123"/>
+      <c r="A37" s="129"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="119"/>
+      <c r="D37" s="119"/>
+      <c r="E37" s="118"/>
       <c r="F37" s="10"/>
     </row>
     <row r="38" spans="1:6" s="21" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="119"/>
-      <c r="B38" s="121"/>
-      <c r="C38" s="121"/>
-      <c r="D38" s="120"/>
-      <c r="E38" s="121"/>
+      <c r="A38" s="114"/>
+      <c r="B38" s="116"/>
+      <c r="C38" s="116"/>
+      <c r="D38" s="115"/>
+      <c r="E38" s="116"/>
       <c r="F38" s="20"/>
     </row>
     <row r="39" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="141"/>
-      <c r="B39" s="123"/>
-      <c r="C39" s="124"/>
-      <c r="D39" s="123"/>
-      <c r="E39" s="123"/>
+      <c r="A39" s="136"/>
+      <c r="B39" s="118"/>
+      <c r="C39" s="119"/>
+      <c r="D39" s="118"/>
+      <c r="E39" s="118"/>
       <c r="F39" s="10"/>
     </row>
     <row r="40" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="157"/>
-      <c r="B40" s="126"/>
-      <c r="C40" s="126"/>
-      <c r="D40" s="127"/>
-      <c r="E40" s="158"/>
+      <c r="A40" s="152"/>
+      <c r="B40" s="121"/>
+      <c r="C40" s="121"/>
+      <c r="D40" s="122"/>
+      <c r="E40" s="153"/>
       <c r="F40" s="85"/>
     </row>
     <row r="41" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="159"/>
-      <c r="B41" s="124"/>
-      <c r="C41" s="124"/>
-      <c r="D41" s="131"/>
-      <c r="E41" s="116"/>
+      <c r="A41" s="154"/>
+      <c r="B41" s="119"/>
+      <c r="C41" s="119"/>
+      <c r="D41" s="126"/>
+      <c r="E41" s="111"/>
       <c r="F41" s="85"/>
     </row>
     <row r="42" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="160"/>
-      <c r="B42" s="120"/>
-      <c r="C42" s="161"/>
-      <c r="D42" s="161"/>
-      <c r="E42" s="162"/>
+      <c r="A42" s="155"/>
+      <c r="B42" s="115"/>
+      <c r="C42" s="156"/>
+      <c r="D42" s="156"/>
+      <c r="E42" s="157"/>
       <c r="F42" s="91"/>
     </row>
     <row r="43" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="163"/>
-      <c r="B43" s="164"/>
-      <c r="C43" s="164"/>
-      <c r="D43" s="165"/>
-      <c r="E43" s="144"/>
+      <c r="A43" s="158"/>
+      <c r="B43" s="159"/>
+      <c r="C43" s="159"/>
+      <c r="D43" s="160"/>
+      <c r="E43" s="139"/>
       <c r="F43" s="93"/>
     </row>
     <row r="44" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="163"/>
-      <c r="B44" s="164"/>
-      <c r="C44" s="164"/>
-      <c r="D44" s="165"/>
-      <c r="E44" s="144"/>
+      <c r="A44" s="158"/>
+      <c r="B44" s="159"/>
+      <c r="C44" s="159"/>
+      <c r="D44" s="160"/>
+      <c r="E44" s="139"/>
       <c r="F44" s="93"/>
     </row>
     <row r="45" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="163"/>
-      <c r="B45" s="164"/>
-      <c r="C45" s="164"/>
-      <c r="D45" s="165"/>
-      <c r="E45" s="144"/>
+      <c r="A45" s="158"/>
+      <c r="B45" s="159"/>
+      <c r="C45" s="159"/>
+      <c r="D45" s="160"/>
+      <c r="E45" s="139"/>
       <c r="F45" s="93"/>
     </row>
     <row r="46" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="163"/>
-      <c r="B46" s="164"/>
-      <c r="C46" s="164"/>
-      <c r="D46" s="165"/>
-      <c r="E46" s="144"/>
+      <c r="A46" s="158"/>
+      <c r="B46" s="159"/>
+      <c r="C46" s="159"/>
+      <c r="D46" s="160"/>
+      <c r="E46" s="139"/>
       <c r="F46" s="93"/>
     </row>
     <row r="47" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="163"/>
-      <c r="B47" s="164"/>
-      <c r="C47" s="164"/>
-      <c r="D47" s="165"/>
-      <c r="E47" s="144"/>
+      <c r="A47" s="158"/>
+      <c r="B47" s="159"/>
+      <c r="C47" s="159"/>
+      <c r="D47" s="160"/>
+      <c r="E47" s="139"/>
       <c r="F47" s="93"/>
     </row>
     <row r="48" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3868,8 +3858,8 @@
   </sheetPr>
   <dimension ref="A3:CJ36"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A10" zoomScale="90" zoomScaleNormal="115" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C36"/>
+    <sheetView view="pageLayout" zoomScale="90" zoomScaleNormal="115" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3884,10 +3874,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:88" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="104" t="s">
+      <c r="C3" s="225" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="104"/>
+      <c r="D3" s="225"/>
     </row>
     <row r="4" spans="1:88" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="2"/>
@@ -3896,8 +3886,8 @@
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
+      <c r="F6" s="224"/>
+      <c r="G6" s="224"/>
     </row>
     <row r="7" spans="1:88" s="26" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
@@ -3998,9 +3988,9 @@
       <c r="CJ7" s="25"/>
     </row>
     <row r="8" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="166"/>
-      <c r="B8" s="167"/>
-      <c r="C8" s="168"/>
+      <c r="A8" s="161"/>
+      <c r="B8" s="162"/>
+      <c r="C8" s="163"/>
       <c r="D8" s="27"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23"/>
@@ -4178,9 +4168,9 @@
       <c r="CJ9" s="25"/>
     </row>
     <row r="10" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="166"/>
-      <c r="B10" s="167"/>
-      <c r="C10" s="169"/>
+      <c r="A10" s="161"/>
+      <c r="B10" s="162"/>
+      <c r="C10" s="164"/>
       <c r="D10" s="28"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
@@ -4268,7 +4258,7 @@
       <c r="CJ10" s="25"/>
     </row>
     <row r="11" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="170"/>
+      <c r="A11" s="165"/>
       <c r="B11" s="11"/>
       <c r="C11" s="7"/>
       <c r="D11" s="28"/>
@@ -4358,7 +4348,7 @@
       <c r="CJ11" s="25"/>
     </row>
     <row r="12" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="171"/>
+      <c r="A12" s="166"/>
       <c r="B12" s="99"/>
       <c r="C12" s="43"/>
       <c r="D12" s="28"/>
@@ -4448,9 +4438,9 @@
       <c r="CJ12" s="25"/>
     </row>
     <row r="13" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="172"/>
-      <c r="B13" s="173"/>
-      <c r="C13" s="168"/>
+      <c r="A13" s="167"/>
+      <c r="B13" s="168"/>
+      <c r="C13" s="163"/>
       <c r="D13" s="29"/>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
@@ -4538,8 +4528,8 @@
       <c r="CJ13" s="25"/>
     </row>
     <row r="14" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="174"/>
-      <c r="B14" s="175"/>
+      <c r="A14" s="169"/>
+      <c r="B14" s="170"/>
       <c r="C14" s="99"/>
       <c r="D14" s="30"/>
       <c r="E14" s="23"/>
@@ -4628,9 +4618,9 @@
       <c r="CJ14" s="25"/>
     </row>
     <row r="15" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="176"/>
-      <c r="B15" s="177"/>
-      <c r="C15" s="168"/>
+      <c r="A15" s="171"/>
+      <c r="B15" s="172"/>
+      <c r="C15" s="163"/>
       <c r="D15" s="31"/>
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
@@ -4718,9 +4708,9 @@
       <c r="CJ15" s="25"/>
     </row>
     <row r="16" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="172"/>
-      <c r="B16" s="167"/>
-      <c r="C16" s="168"/>
+      <c r="A16" s="167"/>
+      <c r="B16" s="162"/>
+      <c r="C16" s="163"/>
       <c r="D16" s="32"/>
       <c r="E16" s="23"/>
       <c r="F16" s="33"/>
@@ -4808,9 +4798,9 @@
       <c r="CJ16" s="25"/>
     </row>
     <row r="17" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="172"/>
-      <c r="B17" s="167"/>
-      <c r="C17" s="167"/>
+      <c r="A17" s="167"/>
+      <c r="B17" s="162"/>
+      <c r="C17" s="162"/>
       <c r="D17" s="32"/>
       <c r="E17" s="23"/>
       <c r="F17" s="33"/>
@@ -4898,7 +4888,7 @@
       <c r="CJ17" s="25"/>
     </row>
     <row r="18" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="178"/>
+      <c r="A18" s="173"/>
       <c r="B18" s="99"/>
       <c r="C18" s="43"/>
       <c r="D18" s="34"/>
@@ -4988,9 +4978,9 @@
       <c r="CJ18" s="25"/>
     </row>
     <row r="19" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="179"/>
-      <c r="B19" s="173"/>
-      <c r="C19" s="180"/>
+      <c r="A19" s="174"/>
+      <c r="B19" s="168"/>
+      <c r="C19" s="175"/>
       <c r="D19" s="35"/>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
@@ -5078,7 +5068,7 @@
       <c r="CJ19" s="25"/>
     </row>
     <row r="20" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="178"/>
+      <c r="A20" s="173"/>
       <c r="B20" s="99"/>
       <c r="C20" s="43"/>
       <c r="D20" s="28"/>
@@ -5168,9 +5158,9 @@
       <c r="CJ20" s="25"/>
     </row>
     <row r="21" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="166"/>
-      <c r="B21" s="167"/>
-      <c r="C21" s="168"/>
+      <c r="A21" s="161"/>
+      <c r="B21" s="162"/>
+      <c r="C21" s="163"/>
       <c r="D21" s="27"/>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
@@ -5258,8 +5248,8 @@
       <c r="CJ21" s="25"/>
     </row>
     <row r="22" spans="1:88" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="181"/>
-      <c r="B22" s="182"/>
+      <c r="A22" s="176"/>
+      <c r="B22" s="177"/>
       <c r="C22" s="99"/>
       <c r="D22" s="19"/>
       <c r="E22" s="36"/>
@@ -5348,9 +5338,9 @@
       <c r="CJ22" s="37"/>
     </row>
     <row r="23" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="166"/>
-      <c r="B23" s="167"/>
-      <c r="C23" s="168"/>
+      <c r="A23" s="161"/>
+      <c r="B23" s="162"/>
+      <c r="C23" s="163"/>
       <c r="D23" s="32"/>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
@@ -5438,9 +5428,9 @@
       <c r="CJ23" s="25"/>
     </row>
     <row r="24" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="172"/>
-      <c r="B24" s="167"/>
-      <c r="C24" s="168"/>
+      <c r="A24" s="167"/>
+      <c r="B24" s="162"/>
+      <c r="C24" s="163"/>
       <c r="D24" s="32"/>
       <c r="E24" s="23"/>
       <c r="F24" s="23"/>
@@ -5528,7 +5518,7 @@
       <c r="CJ24" s="25"/>
     </row>
     <row r="25" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="183"/>
+      <c r="A25" s="178"/>
       <c r="B25" s="11"/>
       <c r="C25" s="7"/>
       <c r="D25" s="28"/>
@@ -5618,9 +5608,9 @@
       <c r="CJ25" s="25"/>
     </row>
     <row r="26" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="166"/>
-      <c r="B26" s="184"/>
-      <c r="C26" s="184"/>
+      <c r="A26" s="161"/>
+      <c r="B26" s="179"/>
+      <c r="C26" s="179"/>
       <c r="D26" s="39"/>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
@@ -5708,9 +5698,9 @@
       <c r="CJ26" s="25"/>
     </row>
     <row r="27" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="185"/>
-      <c r="B27" s="186"/>
-      <c r="C27" s="169"/>
+      <c r="A27" s="180"/>
+      <c r="B27" s="181"/>
+      <c r="C27" s="164"/>
       <c r="D27" s="32"/>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
@@ -5798,7 +5788,7 @@
       <c r="CJ27" s="25"/>
     </row>
     <row r="28" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="170"/>
+      <c r="A28" s="165"/>
       <c r="B28" s="11"/>
       <c r="C28" s="7"/>
       <c r="D28" s="28"/>
@@ -5888,7 +5878,7 @@
       <c r="CJ28" s="25"/>
     </row>
     <row r="29" spans="1:88" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="170"/>
+      <c r="A29" s="165"/>
       <c r="B29" s="11"/>
       <c r="C29" s="7"/>
       <c r="D29" s="28"/>
@@ -6068,9 +6058,9 @@
       <c r="CJ30" s="37"/>
     </row>
     <row r="31" spans="1:88" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="166"/>
-      <c r="B31" s="167"/>
-      <c r="C31" s="168"/>
+      <c r="A31" s="161"/>
+      <c r="B31" s="162"/>
+      <c r="C31" s="163"/>
       <c r="D31" s="28"/>
       <c r="E31" s="36"/>
       <c r="F31" s="36"/>
@@ -6158,9 +6148,9 @@
       <c r="CJ31" s="37"/>
     </row>
     <row r="32" spans="1:88" s="38" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="166"/>
-      <c r="B32" s="167"/>
-      <c r="C32" s="168"/>
+      <c r="A32" s="161"/>
+      <c r="B32" s="162"/>
+      <c r="C32" s="163"/>
       <c r="D32" s="28"/>
       <c r="E32" s="36"/>
       <c r="F32" s="36"/>
@@ -6307,24 +6297,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="103"/>
-      <c r="B2" s="103"/>
-      <c r="C2" s="102" t="s">
+      <c r="A2" s="224"/>
+      <c r="B2" s="224"/>
+      <c r="C2" s="222" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="102"/>
+      <c r="D2" s="222"/>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="103"/>
-      <c r="B3" s="103"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
+      <c r="A3" s="224"/>
+      <c r="B3" s="224"/>
+      <c r="C3" s="222"/>
+      <c r="D3" s="222"/>
     </row>
     <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="105"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
+      <c r="A5" s="226"/>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="226"/>
     </row>
     <row r="7" spans="1:4" s="17" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -6341,189 +6331,189 @@
       </c>
     </row>
     <row r="8" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="187"/>
-      <c r="B8" s="111"/>
-      <c r="C8" s="188"/>
+      <c r="A8" s="182"/>
+      <c r="B8" s="106"/>
+      <c r="C8" s="183"/>
       <c r="D8" s="42"/>
     </row>
     <row r="9" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="189"/>
-      <c r="B9" s="107"/>
-      <c r="C9" s="190"/>
+      <c r="A9" s="184"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="185"/>
       <c r="D9" s="42"/>
     </row>
     <row r="10" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="191"/>
-      <c r="B10" s="192"/>
-      <c r="C10" s="192"/>
+      <c r="A10" s="186"/>
+      <c r="B10" s="187"/>
+      <c r="C10" s="187"/>
       <c r="D10" s="42"/>
     </row>
     <row r="11" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="193"/>
-      <c r="B11" s="194"/>
-      <c r="C11" s="195"/>
+      <c r="A11" s="188"/>
+      <c r="B11" s="189"/>
+      <c r="C11" s="190"/>
       <c r="D11" s="42"/>
     </row>
     <row r="12" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="193"/>
-      <c r="B12" s="196"/>
-      <c r="C12" s="195"/>
+      <c r="A12" s="188"/>
+      <c r="B12" s="191"/>
+      <c r="C12" s="190"/>
       <c r="D12" s="42"/>
     </row>
     <row r="13" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="197"/>
-      <c r="B13" s="192"/>
-      <c r="C13" s="198"/>
+      <c r="A13" s="192"/>
+      <c r="B13" s="187"/>
+      <c r="C13" s="193"/>
       <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="199"/>
-      <c r="B14" s="109"/>
-      <c r="C14" s="200"/>
+      <c r="A14" s="194"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="195"/>
       <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="201"/>
-      <c r="B15" s="109"/>
-      <c r="C15" s="200"/>
+      <c r="A15" s="196"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="195"/>
       <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="201"/>
-      <c r="B16" s="109"/>
-      <c r="C16" s="200"/>
+      <c r="A16" s="196"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="195"/>
       <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="201"/>
-      <c r="B17" s="109"/>
-      <c r="C17" s="200"/>
+      <c r="A17" s="196"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="195"/>
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="193"/>
-      <c r="B18" s="194"/>
-      <c r="C18" s="194"/>
+      <c r="A18" s="188"/>
+      <c r="B18" s="189"/>
+      <c r="C18" s="189"/>
       <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="202"/>
-      <c r="B19" s="202"/>
-      <c r="C19" s="202"/>
+      <c r="A19" s="197"/>
+      <c r="B19" s="197"/>
+      <c r="C19" s="197"/>
       <c r="D19" s="18"/>
     </row>
     <row r="20" spans="1:4" s="46" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="197"/>
-      <c r="B20" s="203"/>
-      <c r="C20" s="204"/>
+      <c r="A20" s="192"/>
+      <c r="B20" s="198"/>
+      <c r="C20" s="199"/>
       <c r="D20" s="45"/>
     </row>
     <row r="21" spans="1:4" s="46" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="205"/>
-      <c r="B21" s="109"/>
-      <c r="C21" s="200"/>
+      <c r="A21" s="200"/>
+      <c r="B21" s="104"/>
+      <c r="C21" s="195"/>
       <c r="D21" s="42"/>
     </row>
     <row r="22" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="193"/>
-      <c r="B22" s="194"/>
-      <c r="C22" s="194"/>
+      <c r="A22" s="188"/>
+      <c r="B22" s="189"/>
+      <c r="C22" s="189"/>
       <c r="D22" s="48"/>
     </row>
     <row r="23" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="191"/>
-      <c r="B23" s="192"/>
-      <c r="C23" s="192"/>
+      <c r="A23" s="186"/>
+      <c r="B23" s="187"/>
+      <c r="C23" s="187"/>
       <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="206"/>
-      <c r="B24" s="202"/>
-      <c r="C24" s="202"/>
+      <c r="A24" s="201"/>
+      <c r="B24" s="197"/>
+      <c r="C24" s="197"/>
       <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="207"/>
-      <c r="B25" s="208"/>
-      <c r="C25" s="195"/>
+      <c r="A25" s="202"/>
+      <c r="B25" s="203"/>
+      <c r="C25" s="190"/>
       <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="205"/>
-      <c r="B26" s="109"/>
-      <c r="C26" s="200"/>
+      <c r="A26" s="200"/>
+      <c r="B26" s="104"/>
+      <c r="C26" s="195"/>
       <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="205"/>
-      <c r="B27" s="109"/>
-      <c r="C27" s="200"/>
+      <c r="A27" s="200"/>
+      <c r="B27" s="104"/>
+      <c r="C27" s="195"/>
       <c r="D27" s="42"/>
     </row>
     <row r="28" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="205"/>
-      <c r="B28" s="109"/>
-      <c r="C28" s="200"/>
+      <c r="A28" s="200"/>
+      <c r="B28" s="104"/>
+      <c r="C28" s="195"/>
       <c r="D28" s="42"/>
     </row>
     <row r="29" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="205"/>
-      <c r="B29" s="109"/>
-      <c r="C29" s="200"/>
+      <c r="A29" s="200"/>
+      <c r="B29" s="104"/>
+      <c r="C29" s="195"/>
       <c r="D29" s="42"/>
     </row>
     <row r="30" spans="1:4" s="14" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="206"/>
-      <c r="B30" s="202"/>
-      <c r="C30" s="202"/>
+      <c r="A30" s="201"/>
+      <c r="B30" s="197"/>
+      <c r="C30" s="197"/>
       <c r="D30" s="42"/>
     </row>
     <row r="31" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="202"/>
-      <c r="B31" s="209"/>
-      <c r="C31" s="209"/>
+      <c r="A31" s="197"/>
+      <c r="B31" s="204"/>
+      <c r="C31" s="204"/>
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="210"/>
-      <c r="B32" s="192"/>
-      <c r="C32" s="192"/>
+      <c r="A32" s="205"/>
+      <c r="B32" s="187"/>
+      <c r="C32" s="187"/>
       <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="210"/>
-      <c r="B33" s="192"/>
-      <c r="C33" s="192"/>
+      <c r="A33" s="205"/>
+      <c r="B33" s="187"/>
+      <c r="C33" s="187"/>
       <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="211"/>
-      <c r="B34" s="212"/>
-      <c r="C34" s="108"/>
+      <c r="A34" s="206"/>
+      <c r="B34" s="207"/>
+      <c r="C34" s="103"/>
       <c r="D34" s="79"/>
     </row>
     <row r="35" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="211"/>
-      <c r="B35" s="212"/>
-      <c r="C35" s="108"/>
+      <c r="A35" s="206"/>
+      <c r="B35" s="207"/>
+      <c r="C35" s="103"/>
       <c r="D35" s="79"/>
     </row>
     <row r="36" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="211"/>
-      <c r="B36" s="212"/>
-      <c r="C36" s="108"/>
+      <c r="A36" s="206"/>
+      <c r="B36" s="207"/>
+      <c r="C36" s="103"/>
       <c r="D36" s="79"/>
     </row>
     <row r="37" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="211"/>
-      <c r="B37" s="212"/>
-      <c r="C37" s="108"/>
+      <c r="A37" s="206"/>
+      <c r="B37" s="207"/>
+      <c r="C37" s="103"/>
       <c r="D37" s="79"/>
     </row>
     <row r="38" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="213"/>
-      <c r="B38" s="214"/>
-      <c r="C38" s="112"/>
+      <c r="A38" s="208"/>
+      <c r="B38" s="209"/>
+      <c r="C38" s="107"/>
       <c r="D38" s="82"/>
     </row>
   </sheetData>
@@ -6553,8 +6543,8 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6568,11 +6558,9 @@
   <sheetData>
     <row r="1" spans="1:9" ht="37" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="49"/>
-      <c r="B1" s="106" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
       <c r="E1" s="50"/>
       <c r="F1" s="50"/>
       <c r="G1" s="50"/>
@@ -6590,22 +6578,24 @@
       <c r="H2" s="50"/>
       <c r="I2" s="50"/>
     </row>
-    <row r="3" spans="1:9" ht="26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="50"/>
       <c r="B3" s="29"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="50"/>
+      <c r="C3" s="228" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="228"/>
       <c r="E3" s="50"/>
       <c r="F3" s="50"/>
       <c r="G3" s="50"/>
       <c r="H3" s="50"/>
       <c r="I3" s="50"/>
     </row>
-    <row r="4" spans="1:9" ht="26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="50"/>
       <c r="B4" s="29"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="50"/>
+      <c r="C4" s="228"/>
+      <c r="D4" s="228"/>
       <c r="E4" s="50"/>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
@@ -6615,8 +6605,8 @@
     <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="50"/>
       <c r="B5" s="29"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
+      <c r="C5" s="228"/>
+      <c r="D5" s="228"/>
       <c r="E5" s="50"/>
       <c r="F5" s="50"/>
       <c r="G5" s="50"/>
@@ -7019,7 +7009,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="C3:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="85" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="2"/>

</xml_diff>